<commit_message>
added kobo python script
</commit_message>
<xml_diff>
--- a/WHOVA2016_v1_5_2_HB_2019_rev4.xlsx
+++ b/WHOVA2016_v1_5_2_HB_2019_rev4.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive\HB 2019 TRAINING\GITHUB\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -18,7 +13,7 @@
   </sheets>
   <definedNames>
     <definedName name="_2016survey">survey!$A$1:$O$609</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$B$1:$B$613</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$Q$1:$Q$613</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5356" uniqueCount="2677">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5353" uniqueCount="2676">
   <si>
     <t>name</t>
   </si>
@@ -7978,9 +7973,6 @@
     <t>select_one select_ethnicity or_other</t>
   </si>
   <si>
-    <t>search</t>
-  </si>
-  <si>
     <t>.&lt;=today()</t>
   </si>
   <si>
@@ -8176,7 +8168,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="37">
     <font>
       <sz val="11"/>
@@ -9084,29 +9076,29 @@
   <dimension ref="A1:Q613"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A548" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C91" sqref="C91"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J71" sqref="J71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.6" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="28.77734375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="58.6640625" style="36" customWidth="1"/>
-    <col min="4" max="4" width="58.33203125" style="36" customWidth="1"/>
-    <col min="5" max="5" width="33.109375" style="36" customWidth="1"/>
-    <col min="6" max="6" width="37.6640625" style="36" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="31.5546875" style="6" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="6" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="6" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="6" customWidth="1"/>
-    <col min="11" max="11" width="28.5546875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="58.7109375" style="36" customWidth="1"/>
+    <col min="4" max="4" width="58.28515625" style="36" customWidth="1"/>
+    <col min="5" max="5" width="33.140625" style="36" customWidth="1"/>
+    <col min="6" max="6" width="37.7109375" style="36" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="31.5703125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="6" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="6" customWidth="1"/>
+    <col min="11" max="11" width="28.5703125" style="6" customWidth="1"/>
     <col min="12" max="12" width="21" style="6" customWidth="1"/>
-    <col min="13" max="13" width="25.33203125" style="6" customWidth="1"/>
-    <col min="14" max="14" width="41.5546875" style="6" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="41.5546875" style="6" customWidth="1"/>
+    <col min="13" max="13" width="25.28515625" style="6" customWidth="1"/>
+    <col min="14" max="14" width="41.5703125" style="6" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="41.5703125" style="6" customWidth="1"/>
     <col min="16" max="16" width="10" style="6" customWidth="1"/>
-    <col min="17" max="16384" width="8.88671875" style="6"/>
+    <col min="17" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.6" customHeight="1">
@@ -9150,7 +9142,7 @@
         <v>9</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>2671</v>
+        <v>2670</v>
       </c>
       <c r="O1" s="6" t="s">
         <v>10</v>
@@ -9159,7 +9151,7 @@
         <v>943</v>
       </c>
       <c r="Q1" s="112" t="s">
-        <v>2655</v>
+        <v>2654</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.6" customHeight="1">
@@ -9451,7 +9443,7 @@
     </row>
     <row r="18" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1">
       <c r="A18" s="114" t="s">
-        <v>2634</v>
+        <v>2633</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>492</v>
@@ -9684,7 +9676,7 @@
         <v>2609</v>
       </c>
       <c r="M30" s="53" t="s">
-        <v>2613</v>
+        <v>2612</v>
       </c>
     </row>
     <row r="31" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -9735,7 +9727,7 @@
         <v>2609</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>2622</v>
+        <v>2621</v>
       </c>
     </row>
     <row r="33" spans="1:15" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -9754,7 +9746,7 @@
       <c r="E33" s="35"/>
       <c r="F33" s="35"/>
       <c r="G33" s="66" t="s">
-        <v>2656</v>
+        <v>2655</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>14</v>
@@ -9763,7 +9755,7 @@
         <v>2609</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>2613</v>
+        <v>2612</v>
       </c>
     </row>
     <row r="34" spans="1:15" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -9811,7 +9803,7 @@
         <v>924</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>2657</v>
+        <v>2656</v>
       </c>
       <c r="N35" s="1" t="s">
         <v>925</v>
@@ -9841,10 +9833,10 @@
         <v>454</v>
       </c>
       <c r="B37" t="s">
+        <v>2640</v>
+      </c>
+      <c r="K37" t="s">
         <v>2641</v>
-      </c>
-      <c r="K37" t="s">
-        <v>2642</v>
       </c>
     </row>
     <row r="38" spans="1:15" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -9939,7 +9931,7 @@
       <c r="E43" s="35"/>
       <c r="F43" s="35"/>
       <c r="K43" t="s">
-        <v>2660</v>
+        <v>2659</v>
       </c>
       <c r="L43" s="5"/>
     </row>
@@ -9955,7 +9947,7 @@
       <c r="E44" s="35"/>
       <c r="F44" s="35"/>
       <c r="K44" t="s">
-        <v>2661</v>
+        <v>2660</v>
       </c>
       <c r="L44" s="5"/>
     </row>
@@ -10038,13 +10030,13 @@
         <v>44</v>
       </c>
       <c r="C48" s="35" t="s">
-        <v>2659</v>
+        <v>2658</v>
       </c>
       <c r="D48" s="109" t="s">
         <v>2010</v>
       </c>
       <c r="E48" t="s">
-        <v>2662</v>
+        <v>2661</v>
       </c>
       <c r="F48" s="35" t="s">
         <v>1868</v>
@@ -10056,13 +10048,13 @@
         <v>14</v>
       </c>
       <c r="M48" s="120" t="s">
-        <v>2658</v>
+        <v>2657</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>2670</v>
+        <v>2669</v>
       </c>
       <c r="O48" s="1" t="s">
-        <v>2670</v>
+        <v>2669</v>
       </c>
     </row>
     <row r="49" spans="1:15" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -10114,7 +10106,7 @@
         <v>2012</v>
       </c>
       <c r="E50" s="40" t="s">
-        <v>2663</v>
+        <v>2662</v>
       </c>
       <c r="F50" s="40" t="s">
         <v>1261</v>
@@ -10609,9 +10601,6 @@
       <c r="H72" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="J72" s="1" t="s">
-        <v>2612</v>
-      </c>
     </row>
     <row r="73" spans="1:11" s="1" customFormat="1" ht="15.6" customHeight="1">
       <c r="A73" s="115" t="s">
@@ -10660,9 +10649,6 @@
       <c r="H74" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J74" s="1" t="s">
-        <v>2612</v>
-      </c>
     </row>
     <row r="75" spans="1:11" s="1" customFormat="1" ht="15.6" customHeight="1">
       <c r="A75" s="1" t="s">
@@ -10726,9 +10712,6 @@
       <c r="H77" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J77" s="1" t="s">
-        <v>2612</v>
-      </c>
     </row>
     <row r="78" spans="1:11" s="1" customFormat="1" ht="15.6" customHeight="1">
       <c r="A78" s="1" t="s">
@@ -10819,7 +10802,7 @@
         <v>2609</v>
       </c>
       <c r="M81" s="66" t="s">
-        <v>2672</v>
+        <v>2671</v>
       </c>
     </row>
     <row r="82" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -11090,7 +11073,7 @@
         <v>14</v>
       </c>
       <c r="J95" s="66" t="s">
-        <v>2664</v>
+        <v>2663</v>
       </c>
     </row>
     <row r="96" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -11150,7 +11133,7 @@
         <v>2609</v>
       </c>
       <c r="M98" t="s">
-        <v>2673</v>
+        <v>2672</v>
       </c>
     </row>
     <row r="99" spans="1:17" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -11227,7 +11210,7 @@
       <c r="E101" s="35"/>
       <c r="F101" s="35"/>
       <c r="K101" s="1" t="s">
-        <v>2620</v>
+        <v>2619</v>
       </c>
     </row>
     <row r="102" spans="1:17" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -11244,7 +11227,7 @@
         <v>2036</v>
       </c>
       <c r="E102" t="s">
-        <v>2665</v>
+        <v>2664</v>
       </c>
       <c r="F102" s="35" t="s">
         <v>1984</v>
@@ -11256,7 +11239,7 @@
         <v>14</v>
       </c>
       <c r="J102" s="66" t="s">
-        <v>2664</v>
+        <v>2663</v>
       </c>
     </row>
     <row r="103" spans="1:17" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -11396,16 +11379,16 @@
     </row>
     <row r="111" spans="1:17" s="115" customFormat="1" ht="15.6" customHeight="1">
       <c r="A111" s="115" t="s">
+        <v>2673</v>
+      </c>
+      <c r="B111" s="115" t="s">
         <v>2674</v>
       </c>
-      <c r="B111" s="115" t="s">
+      <c r="C111" s="115" t="s">
         <v>2675</v>
       </c>
-      <c r="C111" s="115" t="s">
-        <v>2676</v>
-      </c>
       <c r="D111" s="115" t="s">
-        <v>2676</v>
+        <v>2675</v>
       </c>
       <c r="H111" s="115" t="s">
         <v>14</v>
@@ -12409,7 +12392,7 @@
         <v>1432</v>
       </c>
       <c r="D158" t="s">
-        <v>2631</v>
+        <v>2630</v>
       </c>
       <c r="E158" s="35" t="s">
         <v>1869</v>
@@ -12539,7 +12522,7 @@
         <v>1436</v>
       </c>
       <c r="D163" s="109" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
       <c r="E163" s="35"/>
       <c r="F163" s="35"/>
@@ -12570,7 +12553,7 @@
         <v>1437</v>
       </c>
       <c r="D164" s="109" t="s">
-        <v>2630</v>
+        <v>2629</v>
       </c>
       <c r="E164" s="35"/>
       <c r="F164" s="35"/>
@@ -12601,7 +12584,7 @@
         <v>1438</v>
       </c>
       <c r="D165" s="109" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="E165" s="35" t="s">
         <v>937</v>
@@ -14410,7 +14393,7 @@
         <v>2606</v>
       </c>
       <c r="G237" s="115" t="s">
-        <v>2625</v>
+        <v>2624</v>
       </c>
       <c r="H237" s="115" t="s">
         <v>14</v>
@@ -19090,10 +19073,10 @@
         <v>729</v>
       </c>
       <c r="C423" t="s">
+        <v>2625</v>
+      </c>
+      <c r="D423" t="s">
         <v>2626</v>
-      </c>
-      <c r="D423" t="s">
-        <v>2627</v>
       </c>
       <c r="E423"/>
       <c r="F423"/>
@@ -19184,7 +19167,7 @@
         <v>1137</v>
       </c>
       <c r="G427" t="s">
-        <v>2635</v>
+        <v>2634</v>
       </c>
       <c r="M427" s="1" t="s">
         <v>1004</v>
@@ -19207,7 +19190,7 @@
         <v>1684</v>
       </c>
       <c r="D428" t="s">
-        <v>2624</v>
+        <v>2623</v>
       </c>
       <c r="E428" s="35" t="s">
         <v>1126</v>
@@ -19280,7 +19263,7 @@
         <v>113</v>
       </c>
       <c r="G431" t="s">
-        <v>2636</v>
+        <v>2635</v>
       </c>
       <c r="H431" s="1" t="s">
         <v>14</v>
@@ -19302,7 +19285,7 @@
       <c r="E432" s="35"/>
       <c r="F432" s="35"/>
       <c r="G432" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="H432" s="1" t="s">
         <v>14</v>
@@ -19324,7 +19307,7 @@
       <c r="E433" s="35"/>
       <c r="F433" s="35"/>
       <c r="G433" s="119" t="s">
-        <v>2621</v>
+        <v>2620</v>
       </c>
       <c r="H433" s="1" t="s">
         <v>14</v>
@@ -19344,7 +19327,7 @@
         <v>2323</v>
       </c>
       <c r="G434" t="s">
-        <v>2644</v>
+        <v>2643</v>
       </c>
     </row>
     <row r="435" spans="1:15" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -19387,7 +19370,7 @@
         <v>114</v>
       </c>
       <c r="G436" t="s">
-        <v>2645</v>
+        <v>2644</v>
       </c>
       <c r="H436" s="1" t="s">
         <v>14</v>
@@ -19409,7 +19392,7 @@
       <c r="E437" s="35"/>
       <c r="F437" s="35"/>
       <c r="G437" t="s">
-        <v>2646</v>
+        <v>2645</v>
       </c>
       <c r="H437" s="1" t="s">
         <v>14</v>
@@ -19457,7 +19440,7 @@
         <v>989</v>
       </c>
       <c r="G439" t="s">
-        <v>2646</v>
+        <v>2645</v>
       </c>
       <c r="H439" s="1" t="s">
         <v>14</v>
@@ -19510,7 +19493,7 @@
       <c r="E441" s="35"/>
       <c r="F441" s="35"/>
       <c r="G441" t="s">
-        <v>2646</v>
+        <v>2645</v>
       </c>
       <c r="H441" s="1" t="s">
         <v>14</v>
@@ -19532,7 +19515,7 @@
       <c r="E442" s="35"/>
       <c r="F442" s="35"/>
       <c r="G442" t="s">
-        <v>2646</v>
+        <v>2645</v>
       </c>
       <c r="H442" s="1" t="s">
         <v>14</v>
@@ -19554,7 +19537,7 @@
       <c r="E443" s="35"/>
       <c r="F443" s="35"/>
       <c r="G443" t="s">
-        <v>2646</v>
+        <v>2645</v>
       </c>
       <c r="H443" s="1" t="s">
         <v>14</v>
@@ -19576,7 +19559,7 @@
       <c r="E444" s="35"/>
       <c r="F444" s="35"/>
       <c r="G444" t="s">
-        <v>2646</v>
+        <v>2645</v>
       </c>
       <c r="H444" s="1" t="s">
         <v>14</v>
@@ -19598,7 +19581,7 @@
       <c r="E445" s="35"/>
       <c r="F445" s="35"/>
       <c r="G445" t="s">
-        <v>2646</v>
+        <v>2645</v>
       </c>
       <c r="H445" s="1" t="s">
         <v>14</v>
@@ -19672,7 +19655,7 @@
         <v>116</v>
       </c>
       <c r="G448" t="s">
-        <v>2647</v>
+        <v>2646</v>
       </c>
       <c r="H448" s="1" t="s">
         <v>14</v>
@@ -19698,7 +19681,7 @@
         <v>117</v>
       </c>
       <c r="G449" t="s">
-        <v>2648</v>
+        <v>2647</v>
       </c>
       <c r="H449" s="1" t="s">
         <v>14</v>
@@ -19720,7 +19703,7 @@
       <c r="E450" s="35"/>
       <c r="F450" s="35"/>
       <c r="G450" t="s">
-        <v>2647</v>
+        <v>2646</v>
       </c>
       <c r="H450" s="1" t="s">
         <v>14</v>
@@ -19746,7 +19729,7 @@
         <v>118</v>
       </c>
       <c r="G451" t="s">
-        <v>2647</v>
+        <v>2646</v>
       </c>
       <c r="H451" s="1" t="s">
         <v>14</v>
@@ -19772,7 +19755,7 @@
         <v>1146</v>
       </c>
       <c r="G452" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
       <c r="H452" s="16" t="s">
         <v>14</v>
@@ -19866,7 +19849,7 @@
       <c r="E456" s="35"/>
       <c r="F456" s="35"/>
       <c r="G456" t="s">
-        <v>2650</v>
+        <v>2649</v>
       </c>
       <c r="H456" s="1" t="s">
         <v>14</v>
@@ -19883,12 +19866,12 @@
         <v>1977</v>
       </c>
       <c r="D457" t="s">
-        <v>2628</v>
+        <v>2627</v>
       </c>
       <c r="E457" s="35"/>
       <c r="F457" s="35"/>
       <c r="G457" t="s">
-        <v>2651</v>
+        <v>2650</v>
       </c>
       <c r="H457" s="1" t="s">
         <v>14</v>
@@ -19914,7 +19897,7 @@
         <v>1212</v>
       </c>
       <c r="G458" t="s">
-        <v>2651</v>
+        <v>2650</v>
       </c>
       <c r="H458" s="1" t="s">
         <v>14</v>
@@ -19931,12 +19914,12 @@
         <v>1976</v>
       </c>
       <c r="D459" t="s">
-        <v>2629</v>
+        <v>2628</v>
       </c>
       <c r="E459" s="35"/>
       <c r="F459" s="35"/>
       <c r="G459" t="s">
-        <v>2651</v>
+        <v>2650</v>
       </c>
     </row>
     <row r="460" spans="1:15" ht="15.6" customHeight="1">
@@ -19955,7 +19938,7 @@
       <c r="E460" s="35"/>
       <c r="F460" s="35"/>
       <c r="G460" s="6" t="s">
-        <v>2666</v>
+        <v>2665</v>
       </c>
       <c r="H460" s="6" t="s">
         <v>14</v>
@@ -19977,7 +19960,7 @@
       <c r="E461" s="35"/>
       <c r="F461" s="35"/>
       <c r="G461" t="s">
-        <v>2652</v>
+        <v>2651</v>
       </c>
       <c r="H461" s="1" t="s">
         <v>14</v>
@@ -19999,7 +19982,7 @@
       <c r="E462" s="35"/>
       <c r="F462" s="35"/>
       <c r="G462" t="s">
-        <v>2638</v>
+        <v>2637</v>
       </c>
       <c r="H462" s="1" t="s">
         <v>14</v>
@@ -20021,7 +20004,7 @@
       <c r="E463" s="35"/>
       <c r="F463" s="35"/>
       <c r="G463" t="s">
-        <v>2639</v>
+        <v>2638</v>
       </c>
       <c r="H463" s="1" t="s">
         <v>14</v>
@@ -20070,7 +20053,7 @@
       <c r="E467" s="35"/>
       <c r="F467" s="35"/>
       <c r="G467" t="s">
-        <v>2640</v>
+        <v>2639</v>
       </c>
       <c r="H467" s="1" t="s">
         <v>14</v>
@@ -20092,7 +20075,7 @@
       <c r="E468" s="35"/>
       <c r="F468" s="35"/>
       <c r="G468" t="s">
-        <v>2653</v>
+        <v>2652</v>
       </c>
       <c r="H468" s="1" t="s">
         <v>14</v>
@@ -20340,7 +20323,7 @@
         <v>1724</v>
       </c>
       <c r="D478" s="109" t="s">
-        <v>2623</v>
+        <v>2622</v>
       </c>
       <c r="E478" s="35" t="s">
         <v>1186</v>
@@ -20578,7 +20561,7 @@
         <v>2365</v>
       </c>
       <c r="E487" t="s">
-        <v>2667</v>
+        <v>2666</v>
       </c>
       <c r="F487" s="107" t="s">
         <v>1973</v>
@@ -20713,7 +20696,7 @@
         <v>14</v>
       </c>
       <c r="M492" s="121" t="s">
-        <v>2643</v>
+        <v>2642</v>
       </c>
       <c r="N492" s="1" t="s">
         <v>1985</v>
@@ -22920,7 +22903,7 @@
       <c r="E595" s="35"/>
       <c r="F595" s="35"/>
       <c r="G595" s="6" t="s">
-        <v>2669</v>
+        <v>2668</v>
       </c>
     </row>
     <row r="596" spans="1:8" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -23280,7 +23263,6 @@
       <c r="F613" s="17"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B613"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -23291,16 +23273,16 @@
   <dimension ref="A1:G396"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A224" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C324" sqref="C324"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="45.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="45.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="37.33203125" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="45.109375" style="2"/>
+    <col min="1" max="1" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="37.28515625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="45.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="9" customFormat="1">
@@ -24778,7 +24760,7 @@
         <v>1899</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="16.8">
+    <row r="129" spans="1:4" ht="16.5">
       <c r="A129" s="2" t="s">
         <v>195</v>
       </c>
@@ -27331,7 +27313,7 @@
         <v>1228</v>
       </c>
     </row>
-    <row r="341" spans="1:7" ht="16.8">
+    <row r="341" spans="1:7" ht="16.5">
       <c r="A341" s="2" t="s">
         <v>1222</v>
       </c>
@@ -27459,16 +27441,16 @@
     </row>
     <row r="351" spans="1:7">
       <c r="A351" t="s">
+        <v>2613</v>
+      </c>
+      <c r="B351" s="1" t="s">
         <v>2614</v>
       </c>
-      <c r="B351" s="1" t="s">
+      <c r="C351" s="2" t="s">
         <v>2615</v>
       </c>
-      <c r="C351" s="2" t="s">
-        <v>2616</v>
-      </c>
       <c r="D351" s="2" t="s">
-        <v>2616</v>
+        <v>2615</v>
       </c>
       <c r="F351" s="1"/>
       <c r="G351" s="1"/>
@@ -27481,16 +27463,16 @@
     </row>
     <row r="353" spans="1:7">
       <c r="A353" t="s">
+        <v>2616</v>
+      </c>
+      <c r="B353" s="1" t="s">
         <v>2617</v>
       </c>
-      <c r="B353" s="1" t="s">
-        <v>2618</v>
-      </c>
       <c r="C353" s="1" t="s">
-        <v>2618</v>
+        <v>2617</v>
       </c>
       <c r="D353" s="1" t="s">
-        <v>2618</v>
+        <v>2617</v>
       </c>
       <c r="E353" s="1"/>
       <c r="F353" s="1"/>
@@ -27498,16 +27480,16 @@
     </row>
     <row r="354" spans="1:7">
       <c r="A354" t="s">
-        <v>2617</v>
+        <v>2616</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>2619</v>
+        <v>2618</v>
       </c>
       <c r="C354" s="1" t="s">
-        <v>2619</v>
+        <v>2618</v>
       </c>
       <c r="D354" s="1" t="s">
-        <v>2619</v>
+        <v>2618</v>
       </c>
       <c r="E354" s="1"/>
       <c r="F354" s="1"/>
@@ -28080,12 +28062,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="49.44140625" customWidth="1"/>
-    <col min="2" max="2" width="30.5546875" customWidth="1"/>
-    <col min="3" max="3" width="28.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.42578125" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -28107,13 +28089,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>2668</v>
+        <v>2667</v>
       </c>
       <c r="B2" s="25">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>2654</v>
+        <v>2653</v>
       </c>
       <c r="D2" t="s">
         <v>355</v>

</xml_diff>